<commit_message>
Avances sobre los indicadores
Faltan pruebas y correcciones sobre el nuevo parser de indicador. Luego implementar una interfaz para la entrega
</commit_message>
<xml_diff>
--- a/cuentas.xlsx
+++ b/cuentas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Facebook</t>
   </si>
@@ -31,10 +31,16 @@
     <t>Google</t>
   </si>
   <si>
+    <t>INOC</t>
+  </si>
+  <si>
+    <t>UGI's</t>
+  </si>
+  <si>
     <t>FDS</t>
   </si>
   <si>
-    <t>UGI's</t>
+    <t>INOD</t>
   </si>
 </sst>
 </file>
@@ -49,6 +55,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -108,12 +115,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -137,96 +148,95 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="2" t="n">
         <v>2015</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="2" t="n">
         <v>1.34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>2014</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="2" t="n">
         <v>0.83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>2015</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>2.03</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>2016</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="n">
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>0.03</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>2014</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>4.53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>2017</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="n">
+      <c r="B6" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>3.23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalización de los indicadores
Los indicadores ya funcionan según los requisitos: Parsean la fórmula que los define y utilizan las cuentas o los indicadores nombrados por la misma. Falta implementar una interfaz para todo
</commit_message>
<xml_diff>
--- a/cuentas.xlsx
+++ b/cuentas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Facebook</t>
   </si>
@@ -41,14 +41,21 @@
   </si>
   <si>
     <t>INOD</t>
+  </si>
+  <si>
+    <t>DVD</t>
+  </si>
+  <si>
+    <t>CAPT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -115,7 +122,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -126,6 +133,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -145,15 +156,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -181,7 +193,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.83</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,7 +249,36 @@
         <v>6</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>3.23</v>
+        <v>2</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>2014</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>